<commit_message>
completed extracting both times and name file writing completed day12 attendance completed
</commit_message>
<xml_diff>
--- a/sheets/beginner/total.xlsx
+++ b/sheets/beginner/total.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suryan\PycharmProjects\14daysofcode\sheets\beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2F342-245C-4AEC-9670-94B5D9D587E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1591E61-F082-4709-BD15-E5290B955E6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="173">
   <si>
     <t>Bhattakshay13</t>
   </si>
@@ -541,6 +546,9 @@
   </si>
   <si>
     <t>vkt1409</t>
+  </si>
+  <si>
+    <t>mayank403chauhan</t>
   </si>
 </sst>
 </file>
@@ -858,888 +866,2100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A730"/>
+  <dimension ref="A2:D925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A707" workbookViewId="0">
-      <selection activeCell="D724" sqref="D724"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(A$2:A$925,C2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">COUNTIF(A$2:A$925,C3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="1">COUNTIF(A$2:A$925,C67)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>85</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>87</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>89</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>91</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>92</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>93</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>95</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>96</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>97</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>98</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>99</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C103" t="s">
+        <v>101</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
+        <v>102</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C105" t="s">
+        <v>103</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>105</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C108" t="s">
+        <v>106</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C109" t="s">
+        <v>107</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C110" t="s">
+        <v>108</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C111" t="s">
+        <v>109</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C112" t="s">
+        <v>110</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C113" t="s">
+        <v>111</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C114" t="s">
+        <v>112</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C115" t="s">
+        <v>113</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C116" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C117" t="s">
+        <v>115</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C118" t="s">
+        <v>116</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C119" t="s">
+        <v>117</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
+        <v>118</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C121" t="s">
+        <v>119</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C122" t="s">
+        <v>120</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C123" t="s">
+        <v>121</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C124" t="s">
+        <v>122</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C125" t="s">
+        <v>123</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C126" t="s">
+        <v>124</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C127" t="s">
+        <v>125</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C128" t="s">
+        <v>126</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C129" t="s">
+        <v>127</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C130" t="s">
+        <v>128</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C131" t="s">
+        <v>129</v>
+      </c>
+      <c r="D131">
+        <f t="shared" ref="D131:D174" si="2">COUNTIF(A$2:A$925,C131)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C132" t="s">
+        <v>130</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>131</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C134" t="s">
+        <v>132</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C135" t="s">
+        <v>133</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C136" t="s">
+        <v>134</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C137" t="s">
+        <v>135</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C138" t="s">
+        <v>136</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C139" t="s">
+        <v>137</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C140" t="s">
+        <v>138</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C141" t="s">
+        <v>139</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C142" t="s">
+        <v>140</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C143" t="s">
+        <v>141</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C144" t="s">
+        <v>142</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C145" t="s">
+        <v>143</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C146" t="s">
+        <v>144</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>145</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
+        <v>146</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C149" t="s">
+        <v>147</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C150" t="s">
+        <v>148</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C151" t="s">
+        <v>149</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C152" t="s">
+        <v>150</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C153" t="s">
+        <v>151</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C154" t="s">
+        <v>152</v>
+      </c>
+      <c r="D154">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C155" t="s">
+        <v>153</v>
+      </c>
+      <c r="D155">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
+        <v>154</v>
+      </c>
+      <c r="D156">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C157" t="s">
+        <v>155</v>
+      </c>
+      <c r="D157">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C158" t="s">
+        <v>156</v>
+      </c>
+      <c r="D158">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C159" t="s">
+        <v>157</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C160" t="s">
+        <v>158</v>
+      </c>
+      <c r="D160">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C161" t="s">
+        <v>159</v>
+      </c>
+      <c r="D161">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C162" t="s">
+        <v>160</v>
+      </c>
+      <c r="D162">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C163" t="s">
+        <v>161</v>
+      </c>
+      <c r="D163">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C164" t="s">
+        <v>162</v>
+      </c>
+      <c r="D164">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C165" t="s">
+        <v>163</v>
+      </c>
+      <c r="D165">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C166" t="s">
+        <v>164</v>
+      </c>
+      <c r="D166">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C167" t="s">
+        <v>165</v>
+      </c>
+      <c r="D167">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C168" t="s">
+        <v>166</v>
+      </c>
+      <c r="D168">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C169" t="s">
+        <v>167</v>
+      </c>
+      <c r="D169">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C170" t="s">
+        <v>168</v>
+      </c>
+      <c r="D170">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C171" t="s">
+        <v>169</v>
+      </c>
+      <c r="D171">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C172" t="s">
+        <v>170</v>
+      </c>
+      <c r="D172">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C173" t="s">
+        <v>171</v>
+      </c>
+      <c r="D173">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C174" t="s">
+        <v>172</v>
+      </c>
+      <c r="D174">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>84</v>
       </c>
@@ -3766,242 +4986,242 @@
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
-        <v>127</v>
+        <v>42</v>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.3">
@@ -4011,507 +5231,1482 @@
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
-        <v>136</v>
+        <v>53</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
-        <v>146</v>
+        <v>30</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A672" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A684" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A689" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A691" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A696" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
-        <v>157</v>
+        <v>50</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A702" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A704" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A705" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A706" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="707" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
-        <v>163</v>
+        <v>63</v>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
-        <v>164</v>
+        <v>115</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A717" t="s">
-        <v>4</v>
+        <v>148</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A719" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A720" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
     </row>
     <row r="723" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="728" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="729" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="730" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A731" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="732" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A732" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A733" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="734" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A734" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A735" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A736" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="737" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A737" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A738" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="739" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A739" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A740" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A741" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="742" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A742" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A743" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="744" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A744" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A745" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A746" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="747" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A747" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="748" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A748" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="749" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A749" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="750" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A750" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="751" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A751" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="752" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A752" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="753" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A753" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="754" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A754" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A755" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A756" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="757" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A757" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A758" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="759" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A759" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A760" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A761" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="762" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A762" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="763" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A763" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="764" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A764" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A765" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A766" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A767" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A768" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A769" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A770" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A771" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A772" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A773" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A774" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A775" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A776" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A777" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A778" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A779" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A780" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A781" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A782" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A783" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A784" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A785" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A786" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A787" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A788" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A789" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A790" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A791" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A792" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A793" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A794" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A795" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A796" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A797" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A798" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A799" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A800" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A801" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A802" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A803" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A804" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A805" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A806" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A807" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A808" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A809" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A810" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A811" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A812" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A813" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A814" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A815" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A816" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="817" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A817" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A818" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="819" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A819" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A820" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A821" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="822" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A822" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A823" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="824" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A824" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="825" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A825" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="826" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A826" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="827" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A827" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="828" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A828" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="829" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A829" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="830" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A830" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="831" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A831" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="832" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A832" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="833" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A833" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="834" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A834" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="835" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A835" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="836" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A836" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="837" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A837" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="838" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A838" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="839" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A839" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="840" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A840" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="841" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A841" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="842" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A842" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="843" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A843" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="844" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A844" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="845" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A845" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="846" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A846" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="847" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A847" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="848" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A848" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="849" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A849" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="850" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A850" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="851" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A851" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="852" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A852" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="853" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A853" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="854" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A854" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="855" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A855" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="856" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A856" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="857" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A857" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="858" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A858" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="859" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A859" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="860" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A860" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="861" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A861" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="862" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A862" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="863" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A863" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="864" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A864" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="865" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A865" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="866" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A866" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="867" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A867" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="868" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A868" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="869" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A869" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="870" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A870" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="871" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A871" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="872" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A872" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="873" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A873" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="874" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A874" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="875" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A875" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="876" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A876" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A877" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A878" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A879" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A880" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="881" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A881" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="882" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A882" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="883" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A883" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="884" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A884" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="885" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A885" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="886" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A886" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="887" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A887" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="888" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A888" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="889" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A889" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="890" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A890" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="891" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A891" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="892" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A892" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="893" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A893" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="894" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A894" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="895" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A895" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="896" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A896" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="897" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A897" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="898" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A898" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="899" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A899" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="900" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A900" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="901" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A901" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="902" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A902" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="903" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A903" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="904" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A904" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="905" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A905" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A906" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A907" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A908" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A909" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="910" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A910" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="911" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A911" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="912" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A912" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A913" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A914" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A915" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A916" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A917" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A918" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A919" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A920" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A921" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A922" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A923" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A924" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A925" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>